<commit_message>
work on CD41 shp export
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_assainissement_0_4.xlsx
+++ b/Lamia/DBASE/create/Base2_assainissement_0_4.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB113603-F56C-4CF3-AAAF-26CBC2A30252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="3"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -1771,7 +1777,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1984,40 +1990,43 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2066,7 +2075,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2099,9 +2108,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2134,6 +2160,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2309,7 +2352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2700,60 +2743,60 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1"/>
-    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1"/>
-    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1"/>
-    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1"/>
-    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1"/>
-    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1"/>
-    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1"/>
-    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1"/>
-    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1"/>
-    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1"/>
-    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1"/>
-    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1"/>
-    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1"/>
-    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1"/>
-    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1"/>
-    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1"/>
-    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1"/>
-    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1"/>
-    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1"/>
-    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1"/>
-    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1"/>
-    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1"/>
-    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1"/>
-    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1"/>
-    <hyperlink ref="B25" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1"/>
-    <hyperlink ref="B26" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1"/>
-    <hyperlink ref="B27" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1"/>
-    <hyperlink ref="B28" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1"/>
-    <hyperlink ref="B29" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1"/>
-    <hyperlink ref="B30" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1"/>
-    <hyperlink ref="B31" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1"/>
-    <hyperlink ref="B32" location="'10_auth_group'!A1" display="'10_auth_group'!A1"/>
-    <hyperlink ref="B33" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1"/>
-    <hyperlink ref="B34" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1"/>
-    <hyperlink ref="B35" location="'10_auth_user'!A1" display="'10_auth_user'!A1"/>
-    <hyperlink ref="B36" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1"/>
-    <hyperlink ref="B37" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1"/>
-    <hyperlink ref="B38" location="'10_bdd'!A1" display="'10_bdd'!A1"/>
-    <hyperlink ref="B39" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1"/>
-    <hyperlink ref="B40" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1"/>
-    <hyperlink ref="B41" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1"/>
-    <hyperlink ref="B42" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1"/>
-    <hyperlink ref="B43" location="'10_django_session'!A1" display="'10_django_session'!A1"/>
-    <hyperlink ref="B44" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1"/>
-    <hyperlink ref="B45" location="'10_projet'!A1" display="'10_projet'!A1"/>
-    <hyperlink ref="B46" location="'10_siartelia'!A1" display="'10_siartelia'!A1"/>
-    <hyperlink ref="B47" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1"/>
+    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B25" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B26" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B27" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B28" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B29" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B30" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B31" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B32" location="'10_auth_group'!A1" display="'10_auth_group'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B33" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B34" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B35" location="'10_auth_user'!A1" display="'10_auth_user'!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B36" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B37" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B38" location="'10_bdd'!A1" display="'10_bdd'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B39" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B40" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B41" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B42" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B43" location="'10_django_session'!A1" display="'10_django_session'!A1" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B44" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B45" location="'10_projet'!A1" display="'10_projet'!A1" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B46" location="'10_siartelia'!A1" display="'10_siartelia'!A1" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B47" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2836,7 +2879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2921,11 +2964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,7 +3021,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>560</v>
       </c>
       <c r="B3" t="s">
@@ -3136,11 +3179,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3945,7 +3988,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="36" t="s">
+      <c r="A70" s="56" t="s">
         <v>376</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -4372,7 +4415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N138"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4396,7 +4439,7 @@
       <c r="A1" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="19" t="s">
@@ -4419,7 +4462,7 @@
       <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="10" t="s">
@@ -4428,7 +4471,7 @@
       <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="10" t="s">
@@ -4456,13 +4499,13 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>376</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="19" t="s">
@@ -4502,7 +4545,7 @@
       <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4617,7 +4660,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="41" t="s">
         <v>156</v>
       </c>
       <c r="G16" s="10" t="s">
@@ -4673,7 +4716,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="54" t="s">
         <v>342</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -4690,7 +4733,7 @@
       <c r="F21" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="37">
         <v>1</v>
       </c>
       <c r="I21" s="19" t="s">
@@ -4704,7 +4747,7 @@
       <c r="F22" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="37">
         <v>2</v>
       </c>
       <c r="I22" s="19" t="s">
@@ -4718,7 +4761,7 @@
       <c r="F23" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="37">
         <v>3</v>
       </c>
       <c r="I23" s="19" t="s">
@@ -4732,7 +4775,7 @@
       <c r="F24" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="38">
         <v>4</v>
       </c>
       <c r="I24" s="19" t="s">
@@ -4746,7 +4789,7 @@
       <c r="F25" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="38">
         <v>5</v>
       </c>
       <c r="I25" s="19" t="s">
@@ -4760,7 +4803,7 @@
       <c r="F26" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="38">
         <v>6</v>
       </c>
       <c r="I26" s="19" t="s">
@@ -4774,7 +4817,7 @@
       <c r="F27" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="38">
         <v>7</v>
       </c>
       <c r="I27" s="19" t="s">
@@ -4788,7 +4831,7 @@
       <c r="F28" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="G28" s="39">
+      <c r="G28" s="38">
         <v>8</v>
       </c>
       <c r="I28" s="19" t="s">
@@ -4802,7 +4845,7 @@
       <c r="F29" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="39">
+      <c r="G29" s="38">
         <v>0</v>
       </c>
       <c r="I29" s="19" t="s">
@@ -4813,7 +4856,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="50" t="s">
+      <c r="F30" s="49" t="s">
         <v>553</v>
       </c>
       <c r="G30" s="11">
@@ -4830,7 +4873,7 @@
       <c r="F31" s="29" t="s">
         <v>333</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="39">
         <v>20</v>
       </c>
       <c r="I31" s="19" t="s">
@@ -4844,7 +4887,7 @@
       <c r="F32" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="39">
         <v>99</v>
       </c>
       <c r="I32" s="19" t="s">
@@ -4888,32 +4931,32 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="44" t="s">
         <v>147</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I38" s="46" t="s">
+      <c r="I38" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="47" t="s">
+      <c r="J38" s="46" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I39" s="46" t="s">
+      <c r="I39" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="47" t="s">
+      <c r="J39" s="46" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I40" s="46" t="s">
+      <c r="I40" s="45" t="s">
         <v>381</v>
       </c>
-      <c r="J40" s="47" t="s">
+      <c r="J40" s="46" t="s">
         <v>377</v>
       </c>
     </row>
@@ -4930,7 +4973,7 @@
       <c r="C84" s="13"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F88" s="43"/>
+      <c r="F88" s="42"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="13"/>
@@ -4940,33 +4983,33 @@
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="13"/>
-      <c r="F97" s="43"/>
+      <c r="F97" s="42"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="13"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="13"/>
-      <c r="F101" s="43"/>
+      <c r="F101" s="42"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="13"/>
-      <c r="F106" s="43"/>
+      <c r="F106" s="42"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="13"/>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="13"/>
-      <c r="F118" s="43"/>
+      <c r="F118" s="42"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="13"/>
-      <c r="F121" s="43"/>
+      <c r="F121" s="42"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="13"/>
-      <c r="F124" s="43"/>
+      <c r="F124" s="42"/>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="13"/>
@@ -4979,7 +5022,7 @@
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="13"/>
-      <c r="F135" s="43"/>
+      <c r="F135" s="42"/>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138" s="13"/>
@@ -4990,10 +5033,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N219"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
@@ -5254,7 +5297,7 @@
       <c r="G17" s="5">
         <v>62</v>
       </c>
-      <c r="I17" s="49" t="s">
+      <c r="I17" s="48" t="s">
         <v>552</v>
       </c>
       <c r="J17" s="5">
@@ -5384,7 +5427,7 @@
       </c>
     </row>
     <row r="26" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="48" t="s">
         <v>552</v>
       </c>
       <c r="G26" s="5">
@@ -5631,7 +5674,7 @@
       <c r="F51" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="L51" s="41" t="s">
+      <c r="L51" s="40" t="s">
         <v>551</v>
       </c>
       <c r="M51" s="27" t="s">
@@ -5645,7 +5688,7 @@
       <c r="G52" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L52" s="41" t="s">
+      <c r="L52" s="40" t="s">
         <v>550</v>
       </c>
       <c r="M52" s="27" t="s">
@@ -5695,17 +5738,17 @@
       <c r="N56" s="23"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F57" s="51" t="s">
+      <c r="F57" s="50" t="s">
         <v>555</v>
       </c>
-      <c r="G57" s="52" t="s">
+      <c r="G57" s="51" t="s">
         <v>554</v>
       </c>
       <c r="M57" s="23"/>
       <c r="N57" s="23"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F58" s="51"/>
+      <c r="F58" s="50"/>
       <c r="M58" s="23"/>
       <c r="N58" s="23"/>
     </row>
@@ -5779,7 +5822,7 @@
       <c r="N64" s="23"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F65" s="51" t="s">
+      <c r="F65" s="50" t="s">
         <v>556</v>
       </c>
       <c r="G65" s="2" t="s">
@@ -5794,10 +5837,10 @@
       <c r="N65" s="23"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F66" s="53" t="s">
+      <c r="F66" s="52" t="s">
         <v>466</v>
       </c>
-      <c r="G66" s="54" t="s">
+      <c r="G66" s="53" t="s">
         <v>557</v>
       </c>
       <c r="L66" s="19" t="s">
@@ -5953,7 +5996,7 @@
       <c r="L82" s="21"/>
     </row>
     <row r="83" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="37" t="s">
+      <c r="A83" s="36" t="s">
         <v>399</v>
       </c>
       <c r="B83" s="8" t="s">
@@ -6252,7 +6295,7 @@
       <c r="N99" s="11"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="37" t="s">
+      <c r="A100" s="36" t="s">
         <v>401</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -7300,7 +7343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -7454,7 +7497,7 @@
       <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>296</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -7951,7 +7994,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="48" t="s">
+      <c r="A68" s="47" t="s">
         <v>409</v>
       </c>
       <c r="B68" s="34" t="s">

</xml_diff>